<commit_message>
added table cleaning function
</commit_message>
<xml_diff>
--- a/shiny/variables.xlsx
+++ b/shiny/variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projects\Surveys\HHTravel\Survey2017\Data\travel_crosstab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLam\Desktop\travel-study-stories\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7B0F20-71F9-4C02-9B71-3F8442EEBA76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF02DED7-6183-4B9B-A6FE-4C865DBDD475}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29880" yWindow="1185" windowWidth="25980" windowHeight="13005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="person_variables" sheetId="1" r:id="rId1"/>
@@ -370,12 +370,6 @@
     <t>Transit Access Mode</t>
   </si>
   <si>
-    <t>Trip origin Census tract (derived)</t>
-  </si>
-  <si>
-    <t>Trip destination Census tract (derived)</t>
-  </si>
-  <si>
     <t>dest_purpose_simple</t>
   </si>
   <si>
@@ -572,6 +566,12 @@
   </si>
   <si>
     <t>Age 18+_ proxy _ 3_ bike_freq _ 5 days_wk_ Use more bike_ End of trip ammenities</t>
+  </si>
+  <si>
+    <t>o_tract</t>
+  </si>
+  <si>
+    <t>d_tract</t>
   </si>
 </sst>
 </file>
@@ -714,14 +714,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -899,6 +898,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1062,11 +1067,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1425,12 +1431,13 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,7 +1512,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1519,7 +1526,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1575,7 +1582,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -1589,7 +1596,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -1631,10 +1638,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -1645,7 +1652,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="B16" t="s">
         <v>113</v>
@@ -1658,8 +1665,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>117</v>
+      <c r="A17" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="B17" t="s">
         <v>114</v>
@@ -1673,7 +1680,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>115</v>
@@ -1743,7 +1750,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -1757,7 +1764,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -1771,7 +1778,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -1785,7 +1792,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -1799,7 +1806,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -1813,7 +1820,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -1827,7 +1834,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -1841,7 +1848,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -1855,7 +1862,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -1869,7 +1876,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -1911,7 +1918,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1925,7 +1932,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1939,7 +1946,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1953,7 +1960,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1967,7 +1974,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1981,7 +1988,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
         <v>42</v>
@@ -2037,7 +2044,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
         <v>50</v>
@@ -2051,7 +2058,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B45" t="s">
         <v>51</v>
@@ -2093,7 +2100,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
         <v>56</v>
@@ -2107,7 +2114,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
@@ -2121,7 +2128,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
         <v>59</v>
@@ -2135,7 +2142,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B51" t="s">
         <v>60</v>
@@ -2149,7 +2156,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
         <v>61</v>
@@ -2163,7 +2170,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
         <v>62</v>
@@ -2177,7 +2184,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s">
         <v>63</v>
@@ -2191,7 +2198,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
         <v>64</v>
@@ -2205,7 +2212,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B56" t="s">
         <v>65</v>
@@ -2219,7 +2226,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B57" t="s">
         <v>66</v>
@@ -2233,7 +2240,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
         <v>67</v>
@@ -2247,7 +2254,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
         <v>69</v>
@@ -2261,7 +2268,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B60" t="s">
         <v>70</v>
@@ -2275,7 +2282,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B61" t="s">
         <v>71</v>
@@ -2289,7 +2296,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B62" t="s">
         <v>72</v>
@@ -2303,7 +2310,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B63" t="s">
         <v>73</v>
@@ -2317,7 +2324,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B64" t="s">
         <v>74</v>
@@ -2331,7 +2338,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B65" t="s">
         <v>75</v>
@@ -2345,7 +2352,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B66" t="s">
         <v>77</v>
@@ -2359,7 +2366,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B67" t="s">
         <v>78</v>
@@ -2373,7 +2380,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B68" t="s">
         <v>79</v>
@@ -2387,7 +2394,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B69" t="s">
         <v>80</v>
@@ -2401,7 +2408,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
         <v>81</v>
@@ -2415,7 +2422,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B71" t="s">
         <v>83</v>
@@ -2429,7 +2436,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B72" t="s">
         <v>84</v>
@@ -2443,7 +2450,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
         <v>85</v>
@@ -2457,7 +2464,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B74" t="s">
         <v>86</v>
@@ -2471,7 +2478,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B75" t="s">
         <v>87</v>
@@ -2485,7 +2492,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
         <v>88</v>
@@ -2499,7 +2506,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B77" t="s">
         <v>89</v>
@@ -2513,7 +2520,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B78" t="s">
         <v>90</v>
@@ -2527,7 +2534,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B79" t="s">
         <v>91</v>
@@ -2541,7 +2548,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
         <v>92</v>
@@ -2555,7 +2562,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
         <v>93</v>
@@ -2569,7 +2576,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B82" t="s">
         <v>95</v>
@@ -2583,7 +2590,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B83" t="s">
         <v>96</v>
@@ -2597,7 +2604,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B84" t="s">
         <v>97</v>
@@ -2611,7 +2618,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B85" t="s">
         <v>99</v>
@@ -2625,7 +2632,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B86" t="s">
         <v>100</v>
@@ -2639,7 +2646,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B87" t="s">
         <v>101</v>
@@ -2653,7 +2660,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B88" t="s">
         <v>102</v>
@@ -2667,5 +2674,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove detailed geog variables
</commit_message>
<xml_diff>
--- a/shiny/variables.xlsx
+++ b/shiny/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLam\Desktop\travel-study-stories\shiny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travel-study-stories\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E7FCA0-226E-410D-8A9E-F4FD1673BFEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2D505-D426-4527-9659-12305658B5FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="165" windowWidth="27645" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="person_variables" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="249">
   <si>
     <t>Variables</t>
   </si>
@@ -354,12 +354,6 @@
     <t>Mode Group</t>
   </si>
   <si>
-    <t>Trip Origin Tract</t>
-  </si>
-  <si>
-    <t>Trip Destination Tract</t>
-  </si>
-  <si>
     <t>Transit Access Mode</t>
   </si>
   <si>
@@ -555,27 +549,9 @@
     <t>Age 18+_ proxy _ 3_ bike_freq _ 5 days_wk_ Use more bike_ End of trip ammenities</t>
   </si>
   <si>
-    <t>o_tract</t>
-  </si>
-  <si>
-    <t>d_tract</t>
-  </si>
-  <si>
     <t>num_trips</t>
   </si>
   <si>
-    <t>final_home_tract</t>
-  </si>
-  <si>
-    <t>Home Tract</t>
-  </si>
-  <si>
-    <t>final_home_bg</t>
-  </si>
-  <si>
-    <t>Home Block Group</t>
-  </si>
-  <si>
     <t>Part 2 participation group</t>
   </si>
   <si>
@@ -606,66 +582,24 @@
     <t>Rent or Own Home</t>
   </si>
   <si>
-    <t>work_tract</t>
-  </si>
-  <si>
-    <t>Work Tract</t>
-  </si>
-  <si>
-    <t>work_bg</t>
-  </si>
-  <si>
-    <t>Work Block Group</t>
-  </si>
-  <si>
     <t>prev_work_county</t>
   </si>
   <si>
     <t>Previous Work County</t>
   </si>
   <si>
-    <t>prev_work_bg</t>
-  </si>
-  <si>
-    <t>prev_work_tract</t>
-  </si>
-  <si>
-    <t>Previous Work Tract</t>
-  </si>
-  <si>
-    <t>Previous Work Block Group</t>
-  </si>
-  <si>
     <t>school_loc_county</t>
   </si>
   <si>
     <t>School County</t>
   </si>
   <si>
-    <t>school_tract</t>
-  </si>
-  <si>
-    <t>School Tract</t>
-  </si>
-  <si>
     <t>Destination purpose</t>
   </si>
   <si>
     <t>Detailed Purpose</t>
   </si>
   <si>
-    <t>o_bg</t>
-  </si>
-  <si>
-    <t>Trip Destination Block Group</t>
-  </si>
-  <si>
-    <t>Trip Origin Block Group</t>
-  </si>
-  <si>
-    <t>d_bg</t>
-  </si>
-  <si>
     <t>o_rgcname</t>
   </si>
   <si>
@@ -717,12 +651,6 @@
     <t>Usual pay or use a pass to park at work, if usually drive alone or carpool</t>
   </si>
   <si>
-    <t>Work Census Tract</t>
-  </si>
-  <si>
-    <t>Work Census Block Group</t>
-  </si>
-  <si>
     <t>Daily average number of trips</t>
   </si>
   <si>
@@ -747,13 +675,7 @@
     <t>Home County</t>
   </si>
   <si>
-    <t>Home Census Tract</t>
-  </si>
-  <si>
     <t>Type of school attended</t>
-  </si>
-  <si>
-    <t>School Census Tract</t>
   </si>
   <si>
     <t>Household Income Group, in broad categories</t>
@@ -859,7 +781,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -993,12 +915,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1342,12 +1258,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1703,10 +1616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="B47" sqref="A47:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,7 +1646,7 @@
         <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,7 +1697,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1801,7 +1714,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,12 +1731,12 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -1835,12 +1748,12 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -1852,7 +1765,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1869,7 +1782,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1886,7 +1799,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1903,12 +1816,12 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>15</v>
@@ -1920,12 +1833,12 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1937,12 +1850,12 @@
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
@@ -1954,7 +1867,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1971,15 +1884,15 @@
         <v>101</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -1988,15 +1901,15 @@
         <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>175</v>
+      <c r="A17" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>191</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
@@ -2005,15 +1918,15 @@
         <v>101</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>108</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -2022,15 +1935,15 @@
         <v>101</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>208</v>
+        <v>114</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -2039,15 +1952,15 @@
         <v>101</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>211</v>
+        <v>104</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>209</v>
+        <v>105</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
@@ -2056,15 +1969,15 @@
         <v>101</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>212</v>
+        <v>102</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>213</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -2073,15 +1986,15 @@
         <v>101</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>214</v>
+        <v>99</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>215</v>
+        <v>100</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -2090,15 +2003,15 @@
         <v>101</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>116</v>
+        <v>188</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>110</v>
+        <v>189</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -2107,15 +2020,15 @@
         <v>101</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -2124,15 +2037,15 @@
         <v>101</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>102</v>
+        <v>196</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>197</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
@@ -2141,83 +2054,83 @@
         <v>101</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>233</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>206</v>
+        <v>117</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>207</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>216</v>
+        <v>144</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>217</v>
+        <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>219</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>253</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>20</v>
@@ -2226,15 +2139,15 @@
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>20</v>
@@ -2243,15 +2156,15 @@
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>20</v>
@@ -2260,15 +2173,15 @@
         <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>20</v>
@@ -2277,15 +2190,15 @@
         <v>5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>20</v>
@@ -2294,15 +2207,15 @@
         <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>273</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>149</v>
+        <v>30</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>20</v>
@@ -2311,15 +2224,15 @@
         <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>256</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>184</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>27</v>
+        <v>185</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>20</v>
@@ -2328,7 +2241,7 @@
         <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>257</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2336,7 +2249,7 @@
         <v>121</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>20</v>
@@ -2345,7 +2258,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2353,7 +2266,7 @@
         <v>122</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>20</v>
@@ -2362,15 +2275,15 @@
         <v>5</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>29</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>30</v>
+        <v>148</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>20</v>
@@ -2379,15 +2292,15 @@
         <v>5</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>31</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>193</v>
+        <v>35</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>20</v>
@@ -2396,219 +2309,219 @@
         <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>195</v>
+        <v>36</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>197</v>
+        <v>38</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>32</v>
+        <v>181</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>35</v>
+        <v>183</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>202</v>
+        <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>203</v>
+        <v>47</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>204</v>
+        <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>205</v>
+        <v>49</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>186</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>41</v>
@@ -2617,15 +2530,15 @@
         <v>5</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>41</v>
@@ -2634,15 +2547,15 @@
         <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>274</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>40</v>
+        <v>177</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>41</v>
@@ -2651,120 +2564,120 @@
         <v>5</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>238</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>179</v>
+        <v>52</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>181</v>
+        <v>54</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>191</v>
+        <v>56</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>5</v>
@@ -2775,750 +2688,563 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>185</v>
+        <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -3528,12 +3254,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3669,15 +3392,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3760B332-D6CD-416F-8963-74A0770267CF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0DEE16D-DB13-479D-B91F-CA161F8D04BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3701,10 +3428,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0DEE16D-DB13-479D-B91F-CA161F8D04BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3760B332-D6CD-416F-8963-74A0770267CF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
removed the number of trips variable because it is not the average
it's the total number of trips recorded for all household members, across all days
</commit_message>
<xml_diff>
--- a/shiny/variables.xlsx
+++ b/shiny/variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travel-study-stories\shiny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travel-study-stories3\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2D505-D426-4527-9659-12305658B5FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA83BD51-A512-4833-BEA8-2E1318C371A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31455" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="person_variables" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="246">
   <si>
     <t>Variables</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Times used rideshare in past 30 days</t>
   </si>
   <si>
-    <t>Number of Trips</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -549,9 +546,6 @@
     <t>Age 18+_ proxy _ 3_ bike_freq _ 5 days_wk_ Use more bike_ End of trip ammenities</t>
   </si>
   <si>
-    <t>num_trips</t>
-  </si>
-  <si>
     <t>Part 2 participation group</t>
   </si>
   <si>
@@ -649,9 +643,6 @@
   </si>
   <si>
     <t>Usual pay or use a pass to park at work, if usually drive alone or carpool</t>
-  </si>
-  <si>
-    <t>Daily average number of trips</t>
   </si>
   <si>
     <t>Mode Category, in broad groups for sufficient samples for statistical significance</t>
@@ -1616,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
-      <selection activeCell="B47" sqref="A47:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,10 +1634,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1697,7 +1688,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1714,15 +1705,15 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -1731,15 +1722,15 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -1748,12 +1739,12 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -1765,7 +1756,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1782,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1799,7 +1790,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1816,12 +1807,12 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>15</v>
@@ -1833,12 +1824,12 @@
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -1850,58 +1841,58 @@
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>109</v>
+        <v>188</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>110</v>
+        <v>189</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1915,7 +1906,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>191</v>
@@ -1923,84 +1914,84 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>192</v>
+        <v>113</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>99</v>
+        <v>186</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>100</v>
+        <v>187</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>209</v>
@@ -2008,19 +1999,19 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2034,27 +2025,27 @@
         <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>196</v>
+        <v>115</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>197</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2065,30 +2056,30 @@
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2099,13 +2090,13 @@
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2116,13 +2107,13 @@
         <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2133,30 +2124,30 @@
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2167,13 +2158,13 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2184,64 +2175,64 @@
         <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>206</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>182</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>183</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>31</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>185</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2252,47 +2243,47 @@
         <v>32</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2303,13 +2294,13 @@
         <v>35</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2317,50 +2308,50 @@
         <v>124</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>125</v>
+        <v>184</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>38</v>
+        <v>185</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2371,98 +2362,98 @@
         <v>179</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>180</v>
+        <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>42</v>
+        <v>180</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>182</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2473,64 +2464,64 @@
         <v>46</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>217</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>172</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>51</v>
+        <v>173</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2541,30 +2532,30 @@
         <v>175</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>177</v>
+        <v>51</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>177</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2572,16 +2563,16 @@
         <v>128</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="D56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2592,47 +2583,47 @@
         <v>54</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2643,13 +2634,13 @@
         <v>57</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2660,13 +2651,13 @@
         <v>58</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2677,13 +2668,13 @@
         <v>59</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2694,30 +2685,30 @@
         <v>60</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2725,16 +2716,16 @@
         <v>153</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D65" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2745,13 +2736,13 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2762,13 +2753,13 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2779,13 +2770,13 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2796,13 +2787,13 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2813,13 +2804,13 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2830,13 +2821,13 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2844,16 +2835,16 @@
         <v>160</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D72" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,13 +2855,13 @@
         <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2881,13 +2872,13 @@
         <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2898,30 +2889,30 @@
         <v>74</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2929,16 +2920,16 @@
         <v>136</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="D77" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2949,13 +2940,13 @@
         <v>78</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2966,13 +2957,13 @@
         <v>79</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2983,64 +2974,64 @@
         <v>80</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,30 +3042,30 @@
         <v>84</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3085,30 +3076,30 @@
         <v>86</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3116,16 +3107,16 @@
         <v>165</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="D88" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3136,13 +3127,13 @@
         <v>90</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3153,13 +3144,13 @@
         <v>91</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3167,16 +3158,16 @@
         <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="D91" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3187,13 +3178,13 @@
         <v>94</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3204,13 +3195,13 @@
         <v>95</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3221,30 +3212,13 @@
         <v>96</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3254,9 +3228,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3392,19 +3369,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0DEE16D-DB13-479D-B91F-CA161F8D04BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3760B332-D6CD-416F-8963-74A0770267CF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3428,9 +3401,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3760B332-D6CD-416F-8963-74A0770267CF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0DEE16D-DB13-479D-B91F-CA161F8D04BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a8c94ab2-f235-419e-bd5a-9e4b9b75b289"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>